<commit_message>
updates before wrapping up
</commit_message>
<xml_diff>
--- a/Education Outcome Data of Nepal/Educational Outcome Dataset.xlsx
+++ b/Education Outcome Data of Nepal/Educational Outcome Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apanta1/Desktop/Summer Research 2024/Night_Light_Institutional_Capacity/Education Outcome Data of Nepal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC66CDD1-A540-B648-8388-4D71AF94F5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C58684-90C8-CC4F-8707-DFF42F37D928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3200" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{1CC4C0DE-DF3D-43F5-B766-7B2B8BCE34ED}"/>
+    <workbookView xWindow="-3200" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{1CC4C0DE-DF3D-43F5-B766-7B2B8BCE34ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
@@ -5074,7 +5074,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>